<commit_message>
Edit graph stats spreadsheet
</commit_message>
<xml_diff>
--- a/Analysis/graphStats.xlsx
+++ b/Analysis/graphStats.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B302CA84-83CE-4468-B7EF-C58EECF61259}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88112948-446A-40BF-96E0-65FED281D154}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entire Graph" sheetId="1" r:id="rId1"/>
     <sheet name="80s" sheetId="2" r:id="rId2"/>
     <sheet name="90s" sheetId="3" r:id="rId3"/>
     <sheet name="00s" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="78">
   <si>
     <t>Entire Graph</t>
   </si>
   <si>
-    <t>Degree</t>
-  </si>
-  <si>
     <t>Betweenness</t>
   </si>
   <si>
@@ -172,9 +170,6 @@
     <t>EPMD</t>
   </si>
   <si>
-    <t>Ice Cube</t>
-  </si>
-  <si>
     <t>2Pac</t>
   </si>
   <si>
@@ -190,12 +185,6 @@
     <t>KC &amp; the Sunshine Band</t>
   </si>
   <si>
-    <t>Girl Talk</t>
-  </si>
-  <si>
-    <t>Madlib</t>
-  </si>
-  <si>
     <t>Nas</t>
   </si>
   <si>
@@ -230,16 +219,118 @@
   </si>
   <si>
     <t>Marvin Gaye</t>
+  </si>
+  <si>
+    <t>Definitions</t>
+  </si>
+  <si>
+    <t>In-Degree</t>
+  </si>
+  <si>
+    <t>The in-degree centrality for a node v is the fraction of nodes its incoming edges are connected to.</t>
+  </si>
+  <si>
+    <r>
+      <t>Betweenness centrality of a node </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF404040"/>
+        <rFont val="STIXGeneral"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF404040"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>v is the sum of the fraction of all-pairs shortest paths that pass through </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF404040"/>
+        <rFont val="STIXGeneral"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>v</t>
+    </r>
+  </si>
+  <si>
+    <t>Katz centrality computes the relative influence of a node within a network by measuring the number of the immediate neighbors (first degree nodes) and also all other nodes in the network that connect to the node under consideration through these immediate neighbors.</t>
+  </si>
+  <si>
+    <t>Closeness centrality [1] of a node u is the reciprocal of the average shortest path distance to u over all n-1 reachable nodes.</t>
+  </si>
+  <si>
+    <t>PageRank computes a ranking of the nodes in the graph G based on the structure of the incoming links. It was originally designed as an algorithm to rank web pages.</t>
+  </si>
+  <si>
+    <t>Compute the average clustering coefficient for the graph G.</t>
+  </si>
+  <si>
+    <t>the clustering is defined as the fraction of all possible directed triangles</t>
+  </si>
+  <si>
+    <t>Katz, Pagerank, and Eigenvector are all variants of each other</t>
+  </si>
+  <si>
+    <t>Measure of the influence of a node in a network. It assigns relative scores to all nodes in the network based on the concept that connections to high-scoring nodes contribute more to the score of the node in question than equal connections to low-scoring nodes.</t>
+  </si>
+  <si>
+    <t>Betweenness (Random Sample) https://stackoverflow.com/questions/32465503/networkx-never-finishes-calculating-betweenness-centrality-for-2-mil-nodes</t>
+  </si>
+  <si>
+    <t>Eigenvector () https://stackoverflow.com/questions/43208737/using-networkx-to-calculate-eigenvector-centrality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF404040"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF404040"/>
+      <name val="STIXGeneral"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -262,15 +353,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,7 +652,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,41 +677,47 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="1"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>3.1432443703085899E-2</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3">
         <v>4.4770532434783E-3</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3">
         <v>0.103259697072561</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L3">
         <v>0.53245353141680896</v>
@@ -619,25 +725,25 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>1.6263552960800599E-2</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4">
         <v>4.3479265349620601E-3</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4">
         <v>8.5995823833933296E-2</v>
       </c>
       <c r="K4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L4">
         <v>0.22967190973162099</v>
@@ -651,19 +757,19 @@
         <v>1.41784820683903E-2</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5">
         <v>4.1498090373362903E-3</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5">
         <v>7.7975244552604697E-2</v>
       </c>
       <c r="K5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L5">
         <v>0.22423502755208499</v>
@@ -671,25 +777,25 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>1.2145537948290199E-2</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6">
         <v>3.8326758950879801E-3</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6">
         <v>7.7738365340301305E-2</v>
       </c>
       <c r="K6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L6">
         <v>0.18603988345344299</v>
@@ -697,25 +803,25 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>1.07381150959132E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7">
         <v>3.48938623433203E-3</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I7">
         <v>6.7433116339991897E-2</v>
       </c>
       <c r="K7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L7">
         <v>0.17574975177313301</v>
@@ -729,19 +835,19 @@
         <v>1.06338615512927E-2</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8">
         <v>2.3954474688647402E-3</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8">
         <v>6.5938687065384E-2</v>
       </c>
       <c r="K8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L8">
         <v>0.160404183633962</v>
@@ -749,25 +855,25 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>8.6530442035029093E-3</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9">
         <v>2.3604161630464502E-3</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9">
         <v>6.5388505954794396E-2</v>
       </c>
       <c r="K9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L9">
         <v>0.150448904507928</v>
@@ -775,25 +881,25 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>8.4445371142618797E-3</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10">
         <v>1.92803960233274E-3</v>
       </c>
       <c r="H10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I10">
         <v>6.5352496235521002E-2</v>
       </c>
       <c r="K10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L10">
         <v>0.14649736833607699</v>
@@ -801,25 +907,25 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>7.7668890742285199E-3</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11">
         <v>1.75055752964772E-3</v>
       </c>
       <c r="H11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I11">
         <v>6.4875986551251402E-2</v>
       </c>
       <c r="K11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L11">
         <v>0.144001944963459</v>
@@ -827,50 +933,53 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>7.7147623019182604E-3</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12">
         <v>1.7419126230910299E-3</v>
       </c>
       <c r="H12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I12">
         <v>6.3621398195891604E-2</v>
       </c>
       <c r="K12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L12">
         <v>0.138269618666399</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" s="6"/>
+      <c r="H14" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="H14" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>0.47152887007033301</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15">
         <v>1.73748775027243E-2</v>
@@ -881,13 +990,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>0.18032384723036499</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16">
         <v>7.4628979334389004E-3</v>
@@ -895,13 +1004,13 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17">
         <v>0.17249667429482801</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17">
         <v>5.0939674639504297E-3</v>
@@ -909,13 +1018,13 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18">
         <v>0.16527424170017099</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F18">
         <v>4.6953672720655201E-3</v>
@@ -923,13 +1032,13 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>0.13750894445649001</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19">
         <v>4.6491112777755196E-3</v>
@@ -937,13 +1046,13 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20">
         <v>0.134025023140116</v>
       </c>
       <c r="E20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F20">
         <v>4.4441165430597297E-3</v>
@@ -951,13 +1060,13 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21">
         <v>0.117481081963242</v>
       </c>
       <c r="E21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F21">
         <v>4.1158607858129198E-3</v>
@@ -965,13 +1074,13 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <v>0.115831362788647</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F22">
         <v>3.9395490336952901E-3</v>
@@ -979,13 +1088,13 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <v>0.110327211292677</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F23">
         <v>3.80931644671713E-3</v>
@@ -993,13 +1102,13 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>0.109855880585201</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F24">
         <v>3.0994651457239598E-3</v>
@@ -1017,472 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{997B5FF7-DE1D-4633-888E-813840DA9B3C}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.21875" customWidth="1"/>
-    <col min="2" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="3.88671875" customWidth="1"/>
-    <col min="5" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="3.88671875" customWidth="1"/>
-    <col min="8" max="9" width="22.109375" customWidth="1"/>
-    <col min="10" max="10" width="2.6640625" customWidth="1"/>
-    <col min="11" max="12" width="23.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3">
-        <v>8.9091947458595E-2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2">
-        <v>5.1529738108835701E-4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3">
-        <v>0.121669604946241</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3">
-        <v>0.44860030765130299</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>3.8263849229011902E-2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2">
-        <v>3.0513176144244099E-4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4">
-        <v>8.4261946185798894E-2</v>
-      </c>
-      <c r="K4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4">
-        <v>0.39875582902338103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>3.1410622501427697E-2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="2">
-        <v>3.0473470941774701E-4</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5">
-        <v>8.3146257468125803E-2</v>
-      </c>
-      <c r="K5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5">
-        <v>0.39875582902338103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
-        <v>2.74129069103369E-2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2">
-        <v>2.7438470533844598E-4</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6">
-        <v>5.97618304992781E-2</v>
-      </c>
-      <c r="K6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6">
-        <v>0.39875582902338103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>2.2272986864648701E-2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="2">
-        <v>2.5255772211797299E-4</v>
-      </c>
-      <c r="H7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7">
-        <v>5.2262754342578502E-2</v>
-      </c>
-      <c r="K7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7">
-        <v>0.22430015382565199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8">
-        <v>1.94174757281553E-2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="2">
-        <v>2.4441543607734302E-4</v>
-      </c>
-      <c r="H8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8">
-        <v>4.4710143788520999E-2</v>
-      </c>
-      <c r="K8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0.22430015382565199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9">
-        <v>1.6561964591661898E-2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1.3306681896059299E-4</v>
-      </c>
-      <c r="H9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9">
-        <v>4.4573832374531601E-2</v>
-      </c>
-      <c r="K9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0.19937791451169001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10">
-        <v>1.6561964591661898E-2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1.18490114492398E-4</v>
-      </c>
-      <c r="H10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10">
-        <v>3.9089781903412203E-2</v>
-      </c>
-      <c r="K10" t="s">
-        <v>47</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0.19937791451169001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11">
-        <v>1.5990862364363201E-2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="2">
-        <v>9.1104402926219002E-5</v>
-      </c>
-      <c r="H11" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11">
-        <v>3.8514332662037701E-2</v>
-      </c>
-      <c r="K11" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0.19937791451169001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>1.5990862364363201E-2</v>
-      </c>
-      <c r="E12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="2">
-        <v>8.5621821544151595E-5</v>
-      </c>
-      <c r="H12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12">
-        <v>3.82250866343989E-2</v>
-      </c>
-      <c r="K12" t="s">
-        <v>45</v>
-      </c>
-      <c r="L12" s="2">
-        <v>0.19937791451169001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <v>0.38761172233296898</v>
-      </c>
-      <c r="E15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15">
-        <v>5.4940593469867197E-2</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15">
-        <v>4.4707286447255596E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16">
-        <v>0.156466984054071</v>
-      </c>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16">
-        <v>1.69256916791354E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17">
-        <v>0.127037445228251</v>
-      </c>
-      <c r="E17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17">
-        <v>1.6734125256419E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.10646628116613301</v>
-      </c>
-      <c r="E18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18">
-        <v>1.5974369702389399E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19">
-        <v>0.104252367934405</v>
-      </c>
-      <c r="E19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19">
-        <v>1.4040664814384299E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20">
-        <v>8.8094469126809002E-2</v>
-      </c>
-      <c r="E20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20">
-        <v>1.39234969363961E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21">
-        <v>7.8941102500478297E-2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21">
-        <v>1.0726346311192601E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22">
-        <v>7.7605168844295302E-2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22">
-        <v>8.4726259610346105E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23">
-        <v>7.1266313185753105E-2</v>
-      </c>
-      <c r="E23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23">
-        <v>5.7970209902993E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24">
-        <v>7.1144016837589696E-2</v>
-      </c>
-      <c r="E24" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24">
-        <v>5.6928461670996298E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278C6915-0A8D-4694-A9C7-910F50B853FF}">
-  <dimension ref="A1:L24"/>
-  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1503,446 +1148,460 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="K2" t="s">
-        <v>4</v>
       </c>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C3">
-        <v>5.4362722704431203E-2</v>
+        <v>8.7378640776699004E-2</v>
       </c>
       <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5.1529738108835701E-4</v>
+      </c>
+      <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2">
-        <v>7.2484938463900301E-3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
       <c r="I3">
-        <v>0.104227611532774</v>
+        <v>0.121669604946241</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L3">
-        <v>0.54181426007224798</v>
+        <v>0.44860030765130299</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>2.7714329221866899E-2</v>
+        <v>3.7692747001713302E-2</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2">
-        <v>4.7620163174164698E-3</v>
+        <v>3.0513176144244099E-4</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I4">
-        <v>8.6769850570374896E-2</v>
+        <v>8.4261946185798894E-2</v>
       </c>
       <c r="K4" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="L4">
-        <v>0.26879159331917202</v>
+        <v>0.39875582902338103</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>1.9491396375818398E-2</v>
+        <v>2.3986293546544801E-2</v>
       </c>
       <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3.0473470941774701E-4</v>
+      </c>
+      <c r="H5" t="s">
         <v>20</v>
       </c>
-      <c r="F5">
-        <v>3.65149159748212E-3</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
       <c r="I5">
-        <v>7.9254248910724898E-2</v>
+        <v>8.3146257468125803E-2</v>
       </c>
       <c r="K5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L5">
-        <v>0.22200874717142599</v>
+        <v>0.39875582902338103</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>1.5684483021166401E-2</v>
+        <v>2.2272986864648701E-2</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2">
-        <v>3.5777422736661198E-3</v>
+        <v>2.7438470533844598E-4</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="I6">
-        <v>6.12731657888793E-2</v>
+        <v>5.97618304992781E-2</v>
       </c>
       <c r="K6" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="L6">
-        <v>0.198550405710191</v>
+        <v>0.39875582902338103</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C7">
-        <v>1.5684483021166401E-2</v>
+        <v>1.5990862364363201E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2">
-        <v>3.4601986423496902E-3</v>
+        <v>2.5255772211797299E-4</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="I7">
-        <v>6.0145647129137399E-2</v>
+        <v>5.2262754342578502E-2</v>
       </c>
       <c r="K7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L7">
-        <v>0.198388574241461</v>
+        <v>0.22430015382565199</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C8">
-        <v>1.53799299527942E-2</v>
+        <v>1.5990862364363201E-2</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2">
-        <v>3.3479508375095402E-3</v>
+        <v>2.4441543607734302E-4</v>
       </c>
       <c r="H8" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="I8">
-        <v>5.99856327939121E-2</v>
+        <v>4.4710143788520999E-2</v>
       </c>
       <c r="K8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="L8" s="2">
-        <v>0.187022734627628</v>
+        <v>0.22430015382565199</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>1.23343992690726E-2</v>
+        <v>1.5990862364363201E-2</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="F9" s="2">
-        <v>3.19221653822844E-3</v>
+        <v>1.3306681896059299E-4</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9">
-        <v>5.9511562987848501E-2</v>
+        <v>4.4573832374531601E-2</v>
       </c>
       <c r="K9" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="L9" s="2">
-        <v>0.18277501677632699</v>
+        <v>0.19937791451169001</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>1.1573016598142199E-2</v>
+        <v>1.25642490005711E-2</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F10" s="2">
-        <v>2.97777767488033E-3</v>
+        <v>1.18490114492398E-4</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="I10">
-        <v>5.8614763299306399E-2</v>
+        <v>3.9089781903412203E-2</v>
       </c>
       <c r="K10" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="L10" s="2">
-        <v>0.16891086856295701</v>
+        <v>0.19937791451169001</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C11">
-        <v>1.14207400639561E-2</v>
+        <v>1.14220445459737E-2</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="F11" s="2">
-        <v>2.59822658292255E-3</v>
+        <v>9.1104402926219002E-5</v>
       </c>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="I11">
-        <v>5.8570363780625599E-2</v>
+        <v>3.8514332662037701E-2</v>
       </c>
       <c r="K11" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="L11" s="2">
-        <v>0.16848436995786401</v>
+        <v>0.19937791451169001</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C12">
-        <v>1.06593573930257E-2</v>
+        <v>1.0850942318675E-2</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F12" s="2">
-        <v>2.1913915205388199E-3</v>
+        <v>8.5621821544151595E-5</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="I12">
-        <v>5.7257614236054799E-2</v>
+        <v>3.82250866343989E-2</v>
       </c>
       <c r="K12" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="L12" s="2">
-        <v>0.129683985071855</v>
-      </c>
+        <v>0.19937791451169001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E14" t="s">
+      <c r="H14" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="H14" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15">
-        <v>0.42567687951757799</v>
+        <v>0.38761172233296898</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15">
-        <v>2.5108128046272601E-2</v>
+        <v>5.4940593469867197E-2</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15">
-        <v>3.8574235163711399E-3</v>
+        <v>4.4707286447255596E-3</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>0.17592418161044801</v>
+        <v>0.156466984054071</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F16">
-        <v>1.20605542068574E-2</v>
+        <v>1.69256916791354E-2</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17">
-        <v>0.162593722836572</v>
+        <v>0.127037445228251</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
       </c>
       <c r="F17">
-        <v>8.8587499822303899E-3</v>
+        <v>1.6734125256419E-2</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18">
-        <v>0.13196515973516901</v>
+        <v>23</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.10646628116613301</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F18">
-        <v>7.8625504012934198E-3</v>
+        <v>1.5974369702389399E-2</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0.12770826708974001</v>
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>0.104252367934405</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F19">
-        <v>6.6873625119242101E-3</v>
+        <v>1.4040664814384299E-2</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C20">
-        <v>0.107769924704576</v>
+        <v>8.8094469126809002E-2</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F20">
-        <v>5.1682511745576101E-3</v>
+        <v>1.39234969363961E-2</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C21">
-        <v>0.105635683165321</v>
+        <v>7.8941102500478297E-2</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="F21">
-        <v>4.9238157845390802E-3</v>
+        <v>1.0726346311192601E-2</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C22">
-        <v>0.10023740027978099</v>
+        <v>7.7605168844295302E-2</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F22">
-        <v>4.5028583064999402E-3</v>
+        <v>8.4726259610346105E-3</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C23">
-        <v>9.8261122642059898E-2</v>
+        <v>7.1266313185753105E-2</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F23">
-        <v>4.3284819045824197E-3</v>
+        <v>5.7970209902993E-3</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C24">
-        <v>9.4960237014679399E-2</v>
+        <v>7.1144016837589696E-2</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F24">
-        <v>3.0799882028632098E-3</v>
-      </c>
+        <v>5.6928461670996298E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C3FD6D-D78F-4B38-B90E-07CABBCB5C5A}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278C6915-0A8D-4694-A9C7-910F50B853FF}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1959,45 +1618,519 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="K2" t="s">
-        <v>4</v>
       </c>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="C3">
-        <v>1.3046402151983799E-2</v>
+        <v>5.3905893101872999E-2</v>
       </c>
       <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2">
+        <v>7.2484938463900301E-3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <v>0.104227611532774</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3">
+        <v>0.54181426007224798</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>2.2689203593726202E-2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4.7620163174164698E-3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4">
+        <v>8.6769850570374896E-2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4">
+        <v>0.26879159331917202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>1.9491396375818398E-2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <v>3.65149159748212E-3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>7.9254248910724898E-2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5">
+        <v>0.22200874717142599</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>1.5684483021166401E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3.5777422736661198E-3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6">
+        <v>6.12731657888793E-2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6">
+        <v>0.198550405710191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>1.4009441145119501E-2</v>
+      </c>
+      <c r="E7" t="s">
         <v>31</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3.4601986423496902E-3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7">
+        <v>6.0145647129137399E-2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7">
+        <v>0.198388574241461</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1.35526115425612E-2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3.3479508375095402E-3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8">
+        <v>5.99856327939121E-2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.187022734627628</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>1.23343992690726E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3.19221653822844E-3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9">
+        <v>5.9511562987848501E-2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.18277501677632699</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1.05070808588396E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2.97777767488033E-3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10">
+        <v>5.8614763299306399E-2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.16891086856295701</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>1.0202527790467399E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2.59822658292255E-3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11">
+        <v>5.8570363780625599E-2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.16848436995786401</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12">
+        <v>9.2888685853509904E-3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2.1913915205388199E-3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12">
+        <v>5.7257614236054799E-2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.129683985071855</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>0.42567687951757799</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15">
+        <v>2.5108128046272601E-2</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15">
+        <v>3.8574235163711399E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>0.17592418161044801</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16">
+        <v>1.20605542068574E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>0.162593722836572</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <v>8.8587499822303899E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>0.13196515973516901</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18">
+        <v>7.8625504012934198E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.12770826708974001</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19">
+        <v>6.6873625119242101E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>0.107769924704576</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>5.1682511745576101E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>0.105635683165321</v>
+      </c>
+      <c r="E21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21">
+        <v>4.9238157845390802E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22">
+        <v>0.10023740027978099</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22">
+        <v>4.5028583064999402E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23">
+        <v>9.8261122642059898E-2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <v>4.3284819045824197E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>9.4960237014679399E-2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24">
+        <v>3.0799882028632098E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C3FD6D-D78F-4B38-B90E-07CABBCB5C5A}">
+  <dimension ref="A1:L24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="2" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="3.88671875" customWidth="1"/>
+    <col min="5" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="3.88671875" customWidth="1"/>
+    <col min="8" max="9" width="22.109375" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" customWidth="1"/>
+    <col min="11" max="12" width="23.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>9.9529253530598501E-3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
       </c>
       <c r="F3" s="2">
         <v>4.4151636847657697E-4</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3">
         <v>2.7395655690067001E-2</v>
       </c>
       <c r="K3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L3">
         <v>0.34764012244884201</v>
@@ -2005,25 +2138,25 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>9.9529253530598501E-3</v>
+        <v>9.8184263618022807E-3</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="2">
         <v>3.8119234664434298E-4</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4">
         <v>2.5897989889462E-2</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L4">
         <v>0.32771760521151799</v>
@@ -2031,25 +2164,25 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>9.8184263618022807E-3</v>
+        <v>8.2044384667115007E-3</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F5" s="2">
         <v>3.6133230592556002E-4</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I5">
         <v>2.5181582237877399E-2</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L5">
         <v>0.26391655272164999</v>
@@ -2057,25 +2190,25 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>8.2044384667115007E-3</v>
+      </c>
+      <c r="E6" t="s">
         <v>56</v>
-      </c>
-      <c r="C6">
-        <v>9.6839273705447201E-3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>60</v>
       </c>
       <c r="F6" s="2">
         <v>3.2048717799803401E-4</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I6">
         <v>2.43710921974436E-2</v>
       </c>
       <c r="K6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L6">
         <v>0.24879205548648101</v>
@@ -2083,25 +2216,25 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>8.7424344317417607E-3</v>
+        <v>6.8594485541358403E-3</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F7" s="2">
         <v>3.0684248390242701E-4</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I7">
         <v>2.3722831023311099E-2</v>
       </c>
       <c r="K7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L7">
         <v>0.22879683188869801</v>
@@ -2109,25 +2242,25 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>8.7424344317417607E-3</v>
+        <v>5.7834566240753098E-3</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="2">
         <v>2.4142152805255599E-4</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I8">
         <v>2.2286099264395801E-2</v>
       </c>
       <c r="K8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L8" s="2">
         <v>0.20458243131051901</v>
@@ -2135,25 +2268,25 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C9">
-        <v>8.7424344317417607E-3</v>
+        <v>5.7834566240753098E-3</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F9" s="2">
         <v>2.12374462029665E-4</v>
       </c>
       <c r="H9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I9">
         <v>2.2086134264266599E-2</v>
       </c>
       <c r="K9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L9" s="2">
         <v>0.202458423371917</v>
@@ -2161,25 +2294,25 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>8.2044384667115007E-3</v>
+        <v>5.64895763281775E-3</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" s="2">
         <v>1.8351133552939E-4</v>
       </c>
       <c r="H10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I10">
         <v>2.1831482605343799E-2</v>
       </c>
       <c r="K10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L10" s="2">
         <v>0.15531202105945299</v>
@@ -2187,25 +2320,25 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11">
-        <v>7.9354404841963603E-3</v>
+        <v>5.37995965030262E-3</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F11" s="2">
         <v>1.752871280871E-4</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I11">
         <v>2.1332389010404601E-2</v>
       </c>
       <c r="K11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L11" s="2">
         <v>0.15531202105945299</v>
@@ -2213,25 +2346,25 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="C12">
-        <v>7.2629455279085396E-3</v>
+        <v>5.11096166778749E-3</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="2">
         <v>1.7077427743881601E-4</v>
       </c>
       <c r="H12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I12">
         <v>2.07923035508683E-2</v>
       </c>
       <c r="K12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L12" s="2">
         <v>0.15002367961865801</v>
@@ -2241,25 +2374,29 @@
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="H14" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>0.10446151488972701</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15">
         <v>6.5571055280660004E-3</v>
@@ -2271,13 +2408,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>9.89503230518161E-2</v>
       </c>
       <c r="E16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F16">
         <v>3.6758959830177698E-3</v>
@@ -2285,13 +2422,13 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17">
         <v>8.7892444646460205E-2</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F17">
         <v>3.6404151517163202E-3</v>
@@ -2299,13 +2436,13 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1">
         <v>8.3571032468044607E-2</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18">
         <v>3.51948631968905E-3</v>
@@ -2313,13 +2450,13 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19">
         <v>8.1645444681577597E-2</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19">
         <v>3.5136237263023399E-3</v>
@@ -2327,13 +2464,13 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20">
         <v>7.5153374492521602E-2</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F20">
         <v>3.4137545774207199E-3</v>
@@ -2341,13 +2478,13 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21">
         <v>6.4590729425670998E-2</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21">
         <v>2.5714151586089598E-3</v>
@@ -2355,13 +2492,13 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22">
         <v>6.2356757992836499E-2</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F22">
         <v>2.5323652592967199E-3</v>
@@ -2369,13 +2506,13 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C23">
         <v>6.1015988019217302E-2</v>
       </c>
       <c r="E23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F23">
         <v>2.08506196883881E-3</v>
@@ -2383,13 +2520,13 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24">
         <v>5.8201281078116701E-2</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F24">
         <v>1.89497015687394E-3</v>
@@ -2398,4 +2535,108 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9303616-25C6-4F78-87B9-24416B6CB887}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.5">
+      <c r="B5" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" location="id3" display="https://networkx.github.io/documentation/stable/reference/algorithms/generated/networkx.algorithms.centrality.closeness_centrality.html - id3" xr:uid="{A98EA689-C402-491B-A2DD-DE5291323D7D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated paper and images
</commit_message>
<xml_diff>
--- a/Analysis/graphStats.xlsx
+++ b/Analysis/graphStats.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88112948-446A-40BF-96E0-65FED281D154}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E53E8D2-4F2E-45BE-94B8-8659762F5956}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="80s" sheetId="2" r:id="rId2"/>
     <sheet name="90s" sheetId="3" r:id="rId3"/>
     <sheet name="00s" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -652,7 +652,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B2" sqref="B2:L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>